<commit_message>
Updated with the latest Muse barrages (probably)
</commit_message>
<xml_diff>
--- a/BarrageChart.xlsx
+++ b/BarrageChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SICA\Pictures\AL\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79238E16-5F6E-4635-870F-142C5AC6A913}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5745B292-62FB-46D1-89BD-E49097FF58B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="513">
   <si>
     <t>Barrage Name (Skill Level 2)</t>
   </si>
@@ -1500,21 +1500,12 @@
     <t>Fading Memories of Glory</t>
   </si>
   <si>
-    <t>Aulick, Bush, Charles Ausburne, Fletcher, Foote, Hazelwood, Jenkins, Nicholas, Radford, Spence, Thatcher, Kimberly, Mullany, Stanley</t>
-  </si>
-  <si>
     <t>Makinami, Kiyonami</t>
   </si>
   <si>
-    <t>风雨舞踏</t>
-  </si>
-  <si>
     <t>Shigure Kai</t>
   </si>
   <si>
-    <t>四神之印</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -1534,6 +1525,51 @@
   </si>
   <si>
     <t>Buffs the specific Anshan's main gun damage by 16% and strengthens barrage</t>
+  </si>
+  <si>
+    <t>IXB-Class Barrage</t>
+  </si>
+  <si>
+    <t>U-110</t>
+  </si>
+  <si>
+    <t>Dance of Wind and Rain</t>
+  </si>
+  <si>
+    <t>Seal of the Four Gods</t>
+  </si>
+  <si>
+    <t>Aulick, Bush, Charles Ausburne, Fletcher, Foote, Hazelwood, Jenkins, Nicholas, Radford, Spence, Thatcher, Kimberly, Mullany, Stanley, Smalley</t>
+  </si>
+  <si>
+    <t>Cleveland Muse Barrage</t>
+  </si>
+  <si>
+    <t>Sheffield Muse Barrage</t>
+  </si>
+  <si>
+    <t>Sheffield Muse</t>
+  </si>
+  <si>
+    <t>Cleveland Muse</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Akagi Muse</t>
+  </si>
+  <si>
+    <t>Dualism 500lb (3 planes)</t>
+  </si>
+  <si>
+    <t>Dualism 100lb (3 planes)</t>
+  </si>
+  <si>
+    <t>Dualism Torpedo (3 planes)</t>
   </si>
 </sst>
 </file>
@@ -1543,7 +1579,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1680,6 +1716,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1712,7 +1769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1779,6 +1836,9 @@
     <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1920,8 +1980,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Barrage" displayName="Barrage" ref="A1:O126" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:O126" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Barrage" displayName="Barrage" ref="A1:O129" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:O129" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Type"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Barrage Name (Skill Level 2)"/>
@@ -1944,8 +2004,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Barrage4" displayName="Barrage4" ref="A1:U149" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:U149" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Barrage4" displayName="Barrage4" ref="A1:U152" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:U152" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Type"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Skill Name (Max Level)"/>
@@ -2237,10 +2297,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O127"/>
+  <dimension ref="A1:O129"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="O88" sqref="A87:O88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2389,7 +2449,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>489</v>
+        <v>502</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -4189,7 +4249,7 @@
         <v>77</v>
       </c>
       <c r="C52" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D52">
         <v>10</v>
@@ -5522,123 +5582,122 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>132</v>
+        <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>133</v>
+        <v>503</v>
       </c>
       <c r="C87" t="s">
-        <v>135</v>
+        <v>506</v>
       </c>
       <c r="D87">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E87">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F87" s="2">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="G87" s="30">
-        <v>228</v>
-      </c>
-      <c r="H87" s="13" t="s">
-        <v>33</v>
+        <f>Barrage[[#This Row],[Coefficient]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Base Damage]]</f>
+        <v>450</v>
+      </c>
+      <c r="H87" s="10" t="s">
+        <v>508</v>
       </c>
       <c r="I87" s="2">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="J87" s="2">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="K87" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="L87" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="M87" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="L87" s="38"/>
+      <c r="M87" s="39"/>
+      <c r="N87" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>132</v>
+        <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>136</v>
+        <v>504</v>
       </c>
       <c r="C88" t="s">
-        <v>137</v>
+        <v>505</v>
       </c>
       <c r="D88">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E88">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F88" s="2">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="G88" s="30">
-        <v>229</v>
-      </c>
-      <c r="H88" s="13" t="s">
-        <v>33</v>
+        <f>Barrage[[#This Row],[Coefficient]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Base Damage]]</f>
+        <v>600</v>
+      </c>
+      <c r="H88" s="40" t="s">
+        <v>507</v>
       </c>
       <c r="I88" s="2">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="J88" s="2">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="K88" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="L88" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="M88" s="17">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L88" s="38"/>
+      <c r="M88" s="39"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>132</v>
       </c>
       <c r="B89" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C89" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D89">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E89">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F89" s="2">
         <v>1</v>
       </c>
       <c r="G89" s="30">
-        <v>320</v>
-      </c>
-      <c r="H89" t="s">
-        <v>9</v>
+        <v>228</v>
+      </c>
+      <c r="H89" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="I89" s="2">
         <v>1</v>
       </c>
       <c r="J89" s="2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K89" s="2">
-        <v>1</v>
-      </c>
-      <c r="L89" s="15"/>
-      <c r="O89" t="s">
-        <v>57</v>
+        <v>0.6</v>
+      </c>
+      <c r="L89" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M89" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.3">
@@ -5646,25 +5705,25 @@
         <v>132</v>
       </c>
       <c r="B90" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C90" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D90">
         <v>38</v>
       </c>
       <c r="E90">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F90" s="2">
         <v>1</v>
       </c>
       <c r="G90" s="30">
-        <v>304</v>
-      </c>
-      <c r="H90" t="s">
-        <v>9</v>
+        <v>229</v>
+      </c>
+      <c r="H90" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="I90" s="2">
         <v>1</v>
@@ -5675,48 +5734,48 @@
       <c r="K90" s="2">
         <v>0.6</v>
       </c>
-      <c r="L90" s="15"/>
+      <c r="L90" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M90" s="17">
+        <v>2</v>
+      </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>132</v>
       </c>
       <c r="B91" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C91" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D91">
         <v>40</v>
       </c>
       <c r="E91">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F91" s="2">
         <v>1</v>
       </c>
       <c r="G91" s="30">
-        <v>240</v>
-      </c>
-      <c r="H91" s="13" t="s">
-        <v>33</v>
+        <v>320</v>
+      </c>
+      <c r="H91" t="s">
+        <v>9</v>
       </c>
       <c r="I91" s="2">
         <v>1</v>
       </c>
       <c r="J91" s="2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K91" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="L91" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="M91" s="17">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L91" s="15"/>
       <c r="O91" t="s">
         <v>57</v>
       </c>
@@ -5726,25 +5785,25 @@
         <v>132</v>
       </c>
       <c r="B92" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C92" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D92">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E92">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F92" s="2">
         <v>1</v>
       </c>
       <c r="G92" s="30">
-        <v>240</v>
-      </c>
-      <c r="H92" s="13" t="s">
-        <v>33</v>
+        <v>304</v>
+      </c>
+      <c r="H92" t="s">
+        <v>9</v>
       </c>
       <c r="I92" s="2">
         <v>1</v>
@@ -5755,22 +5814,17 @@
       <c r="K92" s="2">
         <v>0.6</v>
       </c>
-      <c r="L92" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="M92" s="17">
-        <v>2</v>
-      </c>
+      <c r="L92" s="15"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>132</v>
       </c>
       <c r="B93" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D93">
         <v>40</v>
@@ -5800,7 +5854,7 @@
         <v>0.3</v>
       </c>
       <c r="M93" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O93" t="s">
         <v>57</v>
@@ -5811,38 +5865,40 @@
         <v>132</v>
       </c>
       <c r="B94" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C94" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D94">
         <v>40</v>
       </c>
       <c r="E94">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F94" s="2">
         <v>1</v>
       </c>
       <c r="G94" s="30">
-        <v>480</v>
-      </c>
-      <c r="H94" s="10" t="s">
-        <v>27</v>
+        <v>240</v>
+      </c>
+      <c r="H94" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="I94" s="2">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J94" s="2">
-        <v>1.1000000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="K94" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="L94" s="15"/>
-      <c r="N94" s="6">
-        <v>1</v>
+        <v>0.6</v>
+      </c>
+      <c r="L94" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M94" s="17">
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.3">
@@ -5850,25 +5906,25 @@
         <v>132</v>
       </c>
       <c r="B95" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C95" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D95">
         <v>40</v>
       </c>
       <c r="E95">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F95" s="2">
         <v>1</v>
       </c>
       <c r="G95" s="30">
-        <v>440</v>
-      </c>
-      <c r="H95" t="s">
-        <v>9</v>
+        <v>240</v>
+      </c>
+      <c r="H95" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="I95" s="2">
         <v>1</v>
@@ -5879,50 +5935,53 @@
       <c r="K95" s="2">
         <v>0.6</v>
       </c>
-      <c r="L95" s="15"/>
+      <c r="L95" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M95" s="17">
+        <v>3</v>
+      </c>
+      <c r="O95" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>132</v>
       </c>
       <c r="B96" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C96" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D96">
         <v>40</v>
       </c>
       <c r="E96">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F96" s="2">
         <v>1</v>
       </c>
       <c r="G96" s="30">
-        <v>240</v>
-      </c>
-      <c r="H96" s="13" t="s">
-        <v>33</v>
+        <v>480</v>
+      </c>
+      <c r="H96" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="I96" s="2">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J96" s="2">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K96" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="L96" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="M96" s="17">
-        <v>1</v>
-      </c>
-      <c r="O96" t="s">
-        <v>57</v>
+        <v>0.75</v>
+      </c>
+      <c r="L96" s="15"/>
+      <c r="N96" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.3">
@@ -5930,22 +5989,22 @@
         <v>132</v>
       </c>
       <c r="B97" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C97" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D97">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E97">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F97" s="2">
         <v>1</v>
       </c>
       <c r="G97" s="30">
-        <v>228</v>
+        <v>440</v>
       </c>
       <c r="H97" t="s">
         <v>9</v>
@@ -5966,22 +6025,22 @@
         <v>132</v>
       </c>
       <c r="B98" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C98" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D98">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E98">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F98" s="2">
         <v>1</v>
       </c>
       <c r="G98" s="30">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="H98" s="13" t="s">
         <v>33</v>
@@ -6000,6 +6059,9 @@
       </c>
       <c r="M98" s="17">
         <v>1</v>
+      </c>
+      <c r="O98" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
@@ -6007,10 +6069,10 @@
         <v>132</v>
       </c>
       <c r="B99" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C99" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D99">
         <v>38</v>
@@ -6043,22 +6105,22 @@
         <v>132</v>
       </c>
       <c r="B100" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C100" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D100">
         <v>38</v>
       </c>
       <c r="E100">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F100" s="2">
         <v>1</v>
       </c>
       <c r="G100" s="30">
-        <v>228</v>
+        <v>190</v>
       </c>
       <c r="H100" s="13" t="s">
         <v>33</v>
@@ -6084,22 +6146,22 @@
         <v>132</v>
       </c>
       <c r="B101" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C101" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D101">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E101">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F101" s="2">
         <v>1</v>
       </c>
       <c r="G101" s="30">
-        <v>540</v>
+        <v>228</v>
       </c>
       <c r="H101" t="s">
         <v>9</v>
@@ -6108,10 +6170,10 @@
         <v>1</v>
       </c>
       <c r="J101" s="2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K101" s="2">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="L101" s="15"/>
     </row>
@@ -6120,43 +6182,40 @@
         <v>132</v>
       </c>
       <c r="B102" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C102" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D102">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E102">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F102" s="2">
         <v>1</v>
       </c>
       <c r="G102" s="30">
-        <v>390</v>
+        <v>228</v>
       </c>
       <c r="H102" s="13" t="s">
         <v>33</v>
       </c>
       <c r="I102" s="2">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="J102" s="2">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="K102" s="2">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="L102" s="15">
-        <v>0.08</v>
+        <v>0.3</v>
       </c>
       <c r="M102" s="17">
-        <v>3</v>
-      </c>
-      <c r="O102" t="s">
-        <v>172</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.3">
@@ -6164,84 +6223,79 @@
         <v>132</v>
       </c>
       <c r="B103" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C103" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D103">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E103">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F103" s="2">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="G103" s="30">
-        <v>528</v>
-      </c>
-      <c r="H103" s="13" t="s">
-        <v>33</v>
+        <v>540</v>
+      </c>
+      <c r="H103" t="s">
+        <v>9</v>
       </c>
       <c r="I103" s="2">
-        <v>1.35</v>
+        <v>1</v>
       </c>
       <c r="J103" s="2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="K103" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="L103" s="15">
-        <v>0.08</v>
-      </c>
-      <c r="M103" s="17">
-        <v>3</v>
-      </c>
-      <c r="O103" t="s">
-        <v>57</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L103" s="15"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>132</v>
       </c>
       <c r="B104" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C104" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D104">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E104">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F104" s="2">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="G104" s="30">
-        <v>501.6</v>
+        <v>390</v>
       </c>
       <c r="H104" s="13" t="s">
         <v>33</v>
       </c>
       <c r="I104" s="2">
-        <v>1.1499999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="J104" s="2">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="K104" s="2">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="L104" s="15">
         <v>0.08</v>
       </c>
       <c r="M104" s="17">
         <v>3</v>
+      </c>
+      <c r="O104" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
@@ -6249,10 +6303,10 @@
         <v>132</v>
       </c>
       <c r="B105" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C105" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D105">
         <v>30</v>
@@ -6266,19 +6320,24 @@
       <c r="G105" s="30">
         <v>528</v>
       </c>
-      <c r="H105" s="10" t="s">
-        <v>27</v>
+      <c r="H105" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="I105" s="2">
-        <v>0.75</v>
+        <v>1.35</v>
       </c>
       <c r="J105" s="2">
-        <v>1.1000000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="K105" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="L105" s="15"/>
+        <v>0.7</v>
+      </c>
+      <c r="L105" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="M105" s="17">
+        <v>3</v>
+      </c>
       <c r="O105" t="s">
         <v>57</v>
       </c>
@@ -6288,43 +6347,40 @@
         <v>132</v>
       </c>
       <c r="B106" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C106" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D106">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E106">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F106" s="2">
         <v>1.1000000000000001</v>
       </c>
       <c r="G106" s="30">
-        <v>528</v>
+        <v>501.6</v>
       </c>
       <c r="H106" s="13" t="s">
         <v>33</v>
       </c>
       <c r="I106" s="2">
-        <v>1.35</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="J106" s="2">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="K106" s="2">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="L106" s="15">
         <v>0.08</v>
       </c>
       <c r="M106" s="17">
         <v>3</v>
-      </c>
-      <c r="O106" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.3">
@@ -6332,41 +6388,36 @@
         <v>132</v>
       </c>
       <c r="B107" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C107" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D107">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E107">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F107" s="2">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G107" s="30">
-        <v>240</v>
-      </c>
-      <c r="H107" s="13" t="s">
-        <v>33</v>
+        <v>528</v>
+      </c>
+      <c r="H107" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="I107" s="2">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J107" s="2">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K107" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="L107" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="M107" s="17">
-        <v>1</v>
-      </c>
+        <v>0.75</v>
+      </c>
+      <c r="L107" s="15"/>
       <c r="O107" t="s">
         <v>57</v>
       </c>
@@ -6376,83 +6427,95 @@
         <v>132</v>
       </c>
       <c r="B108" t="s">
-        <v>363</v>
+        <v>168</v>
       </c>
       <c r="C108" t="s">
-        <v>362</v>
+        <v>169</v>
       </c>
       <c r="D108">
         <v>30</v>
       </c>
       <c r="E108">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F108" s="2">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G108" s="30">
-        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>450</v>
+        <v>528</v>
       </c>
       <c r="H108" s="13" t="s">
         <v>33</v>
       </c>
       <c r="I108" s="2">
-        <v>1.25</v>
+        <v>1.35</v>
       </c>
       <c r="J108" s="2">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="K108" s="2">
-        <v>0.65</v>
-      </c>
-      <c r="L108" s="23"/>
-      <c r="M108" s="24"/>
+        <v>0.7</v>
+      </c>
+      <c r="L108" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="M108" s="17">
+        <v>3</v>
+      </c>
+      <c r="O108" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>132</v>
       </c>
       <c r="B109" t="s">
-        <v>364</v>
+        <v>170</v>
       </c>
       <c r="C109" t="s">
-        <v>362</v>
+        <v>171</v>
       </c>
       <c r="D109">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E109">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F109" s="2">
         <v>1</v>
       </c>
       <c r="G109" s="30">
-        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>525</v>
+        <v>240</v>
       </c>
       <c r="H109" s="13" t="s">
         <v>33</v>
       </c>
       <c r="I109" s="2">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="J109" s="2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K109" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="L109" s="23"/>
-      <c r="M109" s="24"/>
+        <v>0.6</v>
+      </c>
+      <c r="L109" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="M109" s="17">
+        <v>1</v>
+      </c>
+      <c r="O109" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>132</v>
       </c>
       <c r="B110" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C110" t="s">
         <v>362</v>
@@ -6461,120 +6524,121 @@
         <v>30</v>
       </c>
       <c r="E110">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F110" s="2">
         <v>1</v>
       </c>
       <c r="G110" s="30">
         <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>240</v>
-      </c>
-      <c r="H110" s="10" t="s">
-        <v>27</v>
+        <v>450</v>
+      </c>
+      <c r="H110" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="I110" s="2">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="J110" s="2">
-        <v>1.1000000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="K110" s="2">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="L110" s="23"/>
       <c r="M110" s="24"/>
-      <c r="O110" t="s">
-        <v>365</v>
-      </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>132</v>
       </c>
       <c r="B111" t="s">
-        <v>456</v>
+        <v>364</v>
       </c>
       <c r="C111" t="s">
-        <v>457</v>
+        <v>362</v>
       </c>
       <c r="D111">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E111">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F111" s="2">
         <v>1</v>
       </c>
       <c r="G111" s="30">
         <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>252</v>
-      </c>
-      <c r="H111" s="10" t="s">
-        <v>27</v>
+        <v>525</v>
+      </c>
+      <c r="H111" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="I111" s="2">
-        <v>0.85</v>
+        <v>1.25</v>
       </c>
       <c r="J111" s="2">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="K111" s="2">
-        <v>0.85</v>
-      </c>
-      <c r="L111" s="32"/>
-      <c r="M111" s="33"/>
+        <v>0.8</v>
+      </c>
+      <c r="L111" s="23"/>
+      <c r="M111" s="24"/>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>132</v>
       </c>
-      <c r="B112" s="37" t="s">
-        <v>474</v>
+      <c r="B112" t="s">
+        <v>364</v>
       </c>
       <c r="C112" t="s">
-        <v>475</v>
+        <v>362</v>
       </c>
       <c r="D112">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E112">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F112" s="2">
         <v>1</v>
       </c>
       <c r="G112" s="30">
         <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>228</v>
-      </c>
-      <c r="H112" t="s">
-        <v>9</v>
-      </c>
-      <c r="I112">
-        <v>100</v>
+        <v>240</v>
+      </c>
+      <c r="H112" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I112" s="2">
+        <v>0.75</v>
       </c>
       <c r="J112" s="2">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K112" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="L112" s="15"/>
+        <v>0.75</v>
+      </c>
+      <c r="L112" s="23"/>
+      <c r="M112" s="24"/>
+      <c r="O112" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>132</v>
       </c>
       <c r="B113" t="s">
-        <v>476</v>
+        <v>456</v>
       </c>
       <c r="C113" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
       <c r="D113">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E113">
         <v>6</v>
@@ -6584,37 +6648,35 @@
       </c>
       <c r="G113" s="30">
         <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>240</v>
-      </c>
-      <c r="H113" t="s">
-        <v>478</v>
+        <v>252</v>
+      </c>
+      <c r="H113" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="I113" s="2">
-        <v>0.65</v>
+        <v>0.85</v>
       </c>
       <c r="J113" s="2">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="K113" s="2">
-        <v>0.65</v>
-      </c>
-      <c r="L113" s="15"/>
-      <c r="N113" s="6">
-        <v>1</v>
-      </c>
+        <v>0.85</v>
+      </c>
+      <c r="L113" s="32"/>
+      <c r="M113" s="33"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>173</v>
-      </c>
-      <c r="B114" t="s">
-        <v>451</v>
+        <v>132</v>
+      </c>
+      <c r="B114" s="37" t="s">
+        <v>474</v>
       </c>
       <c r="C114" t="s">
-        <v>452</v>
+        <v>475</v>
       </c>
       <c r="D114">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="E114">
         <v>6</v>
@@ -6623,81 +6685,84 @@
         <v>1</v>
       </c>
       <c r="G114" s="30">
-        <v>360</v>
+        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
+        <v>228</v>
       </c>
       <c r="H114" t="s">
-        <v>49</v>
-      </c>
-      <c r="I114" s="2">
+        <v>9</v>
+      </c>
+      <c r="I114">
+        <v>100</v>
+      </c>
+      <c r="J114" s="2">
         <v>0.8</v>
       </c>
-      <c r="J114" s="2">
-        <v>1</v>
-      </c>
       <c r="K114" s="2">
-        <v>1.3</v>
+        <v>0.6</v>
       </c>
       <c r="L114" s="15"/>
-      <c r="M114" s="12"/>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="B115" t="s">
-        <v>174</v>
+        <v>476</v>
       </c>
       <c r="C115" t="s">
-        <v>175</v>
+        <v>477</v>
       </c>
       <c r="D115">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E115">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F115" s="2">
         <v>1</v>
       </c>
       <c r="G115" s="30">
-        <v>540</v>
+        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
+        <v>240</v>
       </c>
       <c r="H115" t="s">
-        <v>49</v>
+        <v>478</v>
       </c>
       <c r="I115" s="2">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="J115" s="2">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="K115" s="2">
-        <v>1.3</v>
+        <v>0.65</v>
       </c>
       <c r="L115" s="15"/>
-      <c r="M115" s="12"/>
+      <c r="N115" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>173</v>
       </c>
       <c r="B116" t="s">
-        <v>181</v>
+        <v>451</v>
       </c>
       <c r="C116" t="s">
-        <v>176</v>
+        <v>452</v>
       </c>
       <c r="D116">
         <v>60</v>
       </c>
       <c r="E116">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F116" s="2">
         <v>1</v>
       </c>
       <c r="G116" s="30">
-        <v>540</v>
+        <v>360</v>
       </c>
       <c r="H116" t="s">
         <v>49</v>
@@ -6719,22 +6784,22 @@
         <v>173</v>
       </c>
       <c r="B117" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C117" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D117">
         <v>60</v>
       </c>
       <c r="E117">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F117" s="2">
         <v>1</v>
       </c>
       <c r="G117" s="30">
-        <v>360</v>
+        <v>540</v>
       </c>
       <c r="H117" t="s">
         <v>49</v>
@@ -6756,23 +6821,22 @@
         <v>173</v>
       </c>
       <c r="B118" t="s">
-        <v>413</v>
+        <v>181</v>
       </c>
       <c r="C118" t="s">
-        <v>414</v>
+        <v>176</v>
       </c>
       <c r="D118">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E118">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F118" s="2">
         <v>1</v>
       </c>
       <c r="G118" s="30">
-        <f>55*6</f>
-        <v>330</v>
+        <v>540</v>
       </c>
       <c r="H118" t="s">
         <v>49</v>
@@ -6786,18 +6850,18 @@
       <c r="K118" s="2">
         <v>1.3</v>
       </c>
-      <c r="L118" s="26"/>
-      <c r="M118" s="28"/>
+      <c r="L118" s="15"/>
+      <c r="M118" s="12"/>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>173</v>
       </c>
       <c r="B119" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C119" t="s">
-        <v>412</v>
+        <v>177</v>
       </c>
       <c r="D119">
         <v>60</v>
@@ -6831,22 +6895,23 @@
         <v>173</v>
       </c>
       <c r="B120" t="s">
-        <v>448</v>
+        <v>413</v>
       </c>
       <c r="C120" t="s">
-        <v>178</v>
+        <v>414</v>
       </c>
       <c r="D120">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E120">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F120" s="2">
         <v>1</v>
       </c>
       <c r="G120" s="30">
-        <v>540</v>
+        <f>55*6</f>
+        <v>330</v>
       </c>
       <c r="H120" t="s">
         <v>49</v>
@@ -6860,71 +6925,67 @@
       <c r="K120" s="2">
         <v>1.3</v>
       </c>
-      <c r="L120" s="15"/>
-      <c r="M120" s="12"/>
+      <c r="L120" s="26"/>
+      <c r="M120" s="28"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>173</v>
       </c>
       <c r="B121" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C121" t="s">
-        <v>179</v>
+        <v>412</v>
       </c>
       <c r="D121">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="E121">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F121" s="2">
         <v>1</v>
       </c>
       <c r="G121" s="30">
-        <v>600</v>
-      </c>
-      <c r="H121" s="13" t="s">
-        <v>33</v>
+        <v>360</v>
+      </c>
+      <c r="H121" t="s">
+        <v>49</v>
       </c>
       <c r="I121" s="2">
-        <v>1.25</v>
+        <v>0.8</v>
       </c>
       <c r="J121" s="2">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="K121" s="2">
-        <v>0.65</v>
-      </c>
-      <c r="L121" s="15">
-        <v>0.08</v>
-      </c>
-      <c r="M121" s="12">
-        <v>3</v>
-      </c>
+        <v>1.3</v>
+      </c>
+      <c r="L121" s="15"/>
+      <c r="M121" s="12"/>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>173</v>
       </c>
       <c r="B122" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="C122" t="s">
-        <v>462</v>
+        <v>178</v>
       </c>
       <c r="D122">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E122">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F122" s="2">
         <v>1</v>
       </c>
       <c r="G122" s="30">
-        <v>576</v>
+        <v>540</v>
       </c>
       <c r="H122" t="s">
         <v>49</v>
@@ -6946,61 +7007,63 @@
         <v>173</v>
       </c>
       <c r="B123" t="s">
-        <v>366</v>
+        <v>184</v>
       </c>
       <c r="C123" t="s">
-        <v>367</v>
+        <v>179</v>
       </c>
       <c r="D123">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="E123">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F123" s="2">
         <v>1</v>
       </c>
       <c r="G123" s="30">
-        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>495</v>
-      </c>
-      <c r="H123" t="s">
-        <v>49</v>
+        <v>600</v>
+      </c>
+      <c r="H123" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="I123" s="2">
-        <v>0.8</v>
+        <v>1.25</v>
       </c>
       <c r="J123" s="2">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="K123" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="L123" s="23"/>
-      <c r="M123" s="25"/>
+        <v>0.65</v>
+      </c>
+      <c r="L123" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="M123" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>173</v>
       </c>
       <c r="B124" t="s">
-        <v>445</v>
+        <v>463</v>
       </c>
       <c r="C124" t="s">
-        <v>444</v>
+        <v>462</v>
       </c>
       <c r="D124">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E124">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F124" s="2">
         <v>1</v>
       </c>
       <c r="G124" s="30">
-        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>540</v>
+        <v>576</v>
       </c>
       <c r="H124" t="s">
         <v>49</v>
@@ -7015,19 +7078,20 @@
         <v>1.3</v>
       </c>
       <c r="L124" s="15"/>
+      <c r="M124" s="12"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>173</v>
       </c>
       <c r="B125" t="s">
-        <v>446</v>
+        <v>366</v>
       </c>
       <c r="C125" t="s">
-        <v>447</v>
+        <v>367</v>
       </c>
       <c r="D125">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E125">
         <v>9</v>
@@ -7037,7 +7101,7 @@
       </c>
       <c r="G125" s="30">
         <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>540</v>
+        <v>495</v>
       </c>
       <c r="H125" t="s">
         <v>49</v>
@@ -7051,30 +7115,31 @@
       <c r="K125" s="2">
         <v>1.3</v>
       </c>
-      <c r="L125" s="15"/>
+      <c r="L125" s="23"/>
+      <c r="M125" s="25"/>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>173</v>
       </c>
       <c r="B126" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C126" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D126">
         <v>60</v>
       </c>
       <c r="E126">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F126" s="2">
         <v>1</v>
       </c>
       <c r="G126" s="30">
         <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>360</v>
+        <v>540</v>
       </c>
       <c r="H126" t="s">
         <v>49</v>
@@ -7091,8 +7156,115 @@
       <c r="L126" s="15"/>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G127" s="30"/>
+      <c r="A127" t="s">
+        <v>173</v>
+      </c>
+      <c r="B127" t="s">
+        <v>446</v>
+      </c>
+      <c r="C127" t="s">
+        <v>447</v>
+      </c>
+      <c r="D127">
+        <v>60</v>
+      </c>
+      <c r="E127">
+        <v>9</v>
+      </c>
+      <c r="F127" s="2">
+        <v>1</v>
+      </c>
+      <c r="G127" s="30">
+        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
+        <v>540</v>
+      </c>
+      <c r="H127" t="s">
+        <v>49</v>
+      </c>
+      <c r="I127" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J127" s="2">
+        <v>1</v>
+      </c>
+      <c r="K127" s="2">
+        <v>1.3</v>
+      </c>
       <c r="L127" s="15"/>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>173</v>
+      </c>
+      <c r="B128" t="s">
+        <v>449</v>
+      </c>
+      <c r="C128" t="s">
+        <v>450</v>
+      </c>
+      <c r="D128">
+        <v>60</v>
+      </c>
+      <c r="E128">
+        <v>6</v>
+      </c>
+      <c r="F128" s="2">
+        <v>1</v>
+      </c>
+      <c r="G128" s="30">
+        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
+        <v>360</v>
+      </c>
+      <c r="H128" t="s">
+        <v>49</v>
+      </c>
+      <c r="I128" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J128" s="2">
+        <v>1</v>
+      </c>
+      <c r="K128" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="L128" s="15"/>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>173</v>
+      </c>
+      <c r="B129" t="s">
+        <v>498</v>
+      </c>
+      <c r="C129" t="s">
+        <v>499</v>
+      </c>
+      <c r="D129">
+        <v>60</v>
+      </c>
+      <c r="E129">
+        <v>6</v>
+      </c>
+      <c r="F129" s="2">
+        <v>1</v>
+      </c>
+      <c r="G129" s="30">
+        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
+        <v>360</v>
+      </c>
+      <c r="H129" t="s">
+        <v>49</v>
+      </c>
+      <c r="I129" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J129" s="2">
+        <v>1</v>
+      </c>
+      <c r="K129" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="L129" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G58">
@@ -7107,7 +7279,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G59:G86">
+  <conditionalFormatting sqref="G59:G88">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -7119,7 +7291,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G87:G113">
+  <conditionalFormatting sqref="G89:G115">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -7131,7 +7303,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G114:G126">
+  <conditionalFormatting sqref="G116:G129">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -7154,10 +7326,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:U166"/>
+  <dimension ref="A1:U169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7226,22 +7398,22 @@
         <v>50</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>496</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -7950,10 +8122,10 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="C20" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D20">
         <v>134</v>
@@ -7987,7 +8159,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
       <c r="C21" t="s">
         <v>60</v>
@@ -8024,7 +8196,7 @@
       <c r="P21" s="12"/>
       <c r="Q21" s="6"/>
       <c r="U21" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
@@ -12192,236 +12364,233 @@
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>332</v>
+        <v>272</v>
       </c>
       <c r="B128" t="s">
-        <v>317</v>
+        <v>510</v>
       </c>
       <c r="C128" t="s">
-        <v>314</v>
+        <v>509</v>
       </c>
       <c r="D128">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="E128">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F128" s="2">
         <v>1</v>
       </c>
       <c r="G128" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>2424</v>
-      </c>
-      <c r="H128" s="9" t="s">
-        <v>301</v>
+        <v>678</v>
+      </c>
+      <c r="H128" t="s">
+        <v>275</v>
       </c>
       <c r="I128" s="2">
         <v>0.8</v>
       </c>
       <c r="J128" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="K128" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K128" s="2">
-        <v>1.3</v>
-      </c>
       <c r="L128" s="15"/>
+      <c r="O128" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>332</v>
+        <v>272</v>
       </c>
       <c r="B129" t="s">
-        <v>316</v>
+        <v>511</v>
       </c>
       <c r="C129" t="s">
-        <v>315</v>
+        <v>509</v>
       </c>
       <c r="D129">
-        <v>240</v>
+        <v>96</v>
       </c>
       <c r="E129">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F129" s="2">
         <v>1</v>
       </c>
       <c r="G129" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>2160</v>
-      </c>
-      <c r="H129" s="9" t="s">
-        <v>301</v>
+        <v>576</v>
+      </c>
+      <c r="H129" t="s">
+        <v>275</v>
       </c>
       <c r="I129" s="2">
         <v>0.8</v>
       </c>
       <c r="J129" s="2">
-        <v>1.1000000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="K129" s="2">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="L129" s="15"/>
+      <c r="O129" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>332</v>
+        <v>272</v>
       </c>
       <c r="B130" t="s">
-        <v>318</v>
+        <v>512</v>
       </c>
       <c r="C130" t="s">
-        <v>319</v>
+        <v>509</v>
       </c>
       <c r="D130">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="E130">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F130" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G130" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>450</v>
-      </c>
-      <c r="H130" s="10" t="s">
-        <v>27</v>
+        <v>1440</v>
+      </c>
+      <c r="H130" t="s">
+        <v>49</v>
       </c>
       <c r="I130" s="2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J130" s="2">
         <v>1</v>
       </c>
       <c r="K130" s="2">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="L130" s="15"/>
-      <c r="O130" t="s">
-        <v>300</v>
-      </c>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>332</v>
       </c>
       <c r="B131" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="C131" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
       <c r="D131">
-        <v>332</v>
+        <v>202</v>
       </c>
       <c r="E131">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F131" s="2">
         <v>1</v>
       </c>
       <c r="G131" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>332</v>
+        <v>2424</v>
       </c>
       <c r="H131" s="9" t="s">
-        <v>275</v>
+        <v>301</v>
       </c>
       <c r="I131" s="2">
         <v>0.8</v>
       </c>
       <c r="J131" s="2">
-        <v>0.95</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K131" s="2">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="L131" s="15"/>
-      <c r="O131" t="s">
-        <v>281</v>
-      </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>332</v>
       </c>
       <c r="B132" t="s">
-        <v>342</v>
+        <v>316</v>
       </c>
       <c r="C132" t="s">
-        <v>340</v>
+        <v>315</v>
       </c>
       <c r="D132">
-        <v>138</v>
+        <v>240</v>
       </c>
       <c r="E132">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F132" s="2">
         <v>1</v>
       </c>
       <c r="G132" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>276</v>
+        <v>2160</v>
       </c>
       <c r="H132" s="9" t="s">
-        <v>275</v>
+        <v>301</v>
       </c>
       <c r="I132" s="2">
         <v>0.8</v>
       </c>
       <c r="J132" s="2">
-        <v>0.85</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K132" s="2">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="L132" s="15"/>
-      <c r="O132" t="s">
-        <v>281</v>
-      </c>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>332</v>
       </c>
       <c r="B133" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="C133" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="D133">
-        <v>288</v>
+        <v>225</v>
       </c>
       <c r="E133">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F133" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G133" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>1728</v>
-      </c>
-      <c r="H133" s="9" t="s">
-        <v>286</v>
+        <v>450</v>
+      </c>
+      <c r="H133" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="I133" s="2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J133" s="2">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="K133" s="2">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="L133" s="15"/>
       <c r="O133" t="s">
-        <v>281</v>
+        <v>300</v>
       </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.3">
@@ -12429,118 +12598,119 @@
         <v>332</v>
       </c>
       <c r="B134" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="C134" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="D134">
-        <v>207</v>
+        <v>332</v>
       </c>
       <c r="E134">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F134" s="2">
         <v>1</v>
       </c>
       <c r="G134" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>621</v>
-      </c>
-      <c r="H134" t="s">
-        <v>49</v>
+        <v>332</v>
+      </c>
+      <c r="H134" s="9" t="s">
+        <v>275</v>
       </c>
       <c r="I134" s="2">
         <v>0.8</v>
       </c>
       <c r="J134" s="2">
-        <v>1.1000000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="K134" s="2">
-        <v>1.3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="L134" s="15"/>
+      <c r="O134" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>332</v>
       </c>
       <c r="B135" t="s">
-        <v>442</v>
+        <v>342</v>
       </c>
       <c r="C135" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="D135">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="E135">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F135" s="2">
         <v>1</v>
       </c>
       <c r="G135" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>1242</v>
-      </c>
-      <c r="H135" t="s">
-        <v>49</v>
+        <v>276</v>
+      </c>
+      <c r="H135" s="9" t="s">
+        <v>275</v>
       </c>
       <c r="I135" s="2">
         <v>0.8</v>
       </c>
       <c r="J135" s="2">
-        <v>1.1000000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="K135" s="2">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="L135" s="15"/>
+      <c r="O135" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>332</v>
       </c>
       <c r="B136" t="s">
-        <v>423</v>
+        <v>338</v>
       </c>
       <c r="C136" t="s">
-        <v>424</v>
+        <v>339</v>
       </c>
       <c r="D136">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E136">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F136" s="2">
         <v>1</v>
       </c>
       <c r="G136" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>294</v>
-      </c>
-      <c r="H136" s="13" t="s">
-        <v>299</v>
+        <v>1728</v>
+      </c>
+      <c r="H136" s="9" t="s">
+        <v>286</v>
       </c>
       <c r="I136" s="2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J136" s="2">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K136" s="2">
-        <v>1</v>
-      </c>
-      <c r="L136" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="M136" s="27">
-        <v>3</v>
-      </c>
+        <v>1.3</v>
+      </c>
+      <c r="L136" s="15"/>
       <c r="O136" t="s">
-        <v>425</v>
+        <v>281</v>
       </c>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.3">
@@ -12548,13 +12718,13 @@
         <v>332</v>
       </c>
       <c r="B137" t="s">
-        <v>423</v>
+        <v>348</v>
       </c>
       <c r="C137" t="s">
-        <v>424</v>
+        <v>349</v>
       </c>
       <c r="D137">
-        <v>248</v>
+        <v>207</v>
       </c>
       <c r="E137">
         <v>3</v>
@@ -12564,239 +12734,242 @@
       </c>
       <c r="G137" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>744</v>
-      </c>
-      <c r="H137" s="10" t="s">
-        <v>426</v>
+        <v>621</v>
+      </c>
+      <c r="H137" t="s">
+        <v>49</v>
       </c>
       <c r="I137" s="2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J137" s="2">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K137" s="2">
-        <v>1</v>
-      </c>
-      <c r="L137" s="26"/>
-      <c r="M137" s="27"/>
+        <v>1.3</v>
+      </c>
+      <c r="L137" s="15"/>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>332</v>
       </c>
       <c r="B138" t="s">
-        <v>423</v>
+        <v>442</v>
       </c>
       <c r="C138" t="s">
-        <v>424</v>
+        <v>349</v>
       </c>
       <c r="D138">
-        <v>72</v>
+        <v>207</v>
       </c>
       <c r="E138">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="F138" s="2">
         <v>1</v>
       </c>
       <c r="G138" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>1728</v>
+        <v>1242</v>
       </c>
       <c r="H138" t="s">
-        <v>275</v>
+        <v>49</v>
       </c>
       <c r="I138" s="2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J138" s="2">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K138" s="2">
-        <v>1</v>
-      </c>
-      <c r="L138" s="26"/>
-      <c r="M138" s="27"/>
+        <v>1.3</v>
+      </c>
+      <c r="L138" s="15"/>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>332</v>
       </c>
       <c r="B139" t="s">
-        <v>468</v>
+        <v>423</v>
       </c>
       <c r="C139" t="s">
-        <v>464</v>
+        <v>424</v>
       </c>
       <c r="D139">
-        <v>380</v>
+        <v>294</v>
       </c>
       <c r="E139">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F139" s="2">
         <v>1</v>
       </c>
       <c r="G139" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>2280</v>
-      </c>
-      <c r="H139" t="s">
-        <v>275</v>
+        <v>294</v>
+      </c>
+      <c r="H139" s="13" t="s">
+        <v>299</v>
       </c>
       <c r="I139" s="2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J139" s="2">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K139" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="L139" s="15"/>
-      <c r="M139" s="12"/>
+        <v>1</v>
+      </c>
+      <c r="L139" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="M139" s="27">
+        <v>3</v>
+      </c>
+      <c r="O139" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B140" t="s">
-        <v>359</v>
+        <v>423</v>
       </c>
       <c r="C140" t="s">
-        <v>360</v>
+        <v>424</v>
       </c>
       <c r="D140">
-        <v>173</v>
+        <v>248</v>
       </c>
       <c r="E140">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F140" s="2">
         <v>1</v>
       </c>
       <c r="G140" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>2595</v>
-      </c>
-      <c r="H140" t="s">
-        <v>275</v>
+        <v>744</v>
+      </c>
+      <c r="H140" s="10" t="s">
+        <v>426</v>
       </c>
       <c r="I140" s="2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J140" s="2">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="K140" s="2">
         <v>1</v>
       </c>
-      <c r="L140" s="15"/>
-      <c r="O140" t="s">
-        <v>281</v>
-      </c>
+      <c r="L140" s="26"/>
+      <c r="M140" s="27"/>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B141" t="s">
-        <v>321</v>
+        <v>423</v>
       </c>
       <c r="C141" t="s">
-        <v>320</v>
+        <v>424</v>
       </c>
       <c r="D141">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="E141">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F141" s="2">
         <v>1</v>
       </c>
       <c r="G141" s="30">
-        <v>800</v>
-      </c>
-      <c r="H141" s="13" t="s">
-        <v>33</v>
+        <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
+        <v>1728</v>
+      </c>
+      <c r="H141" t="s">
+        <v>275</v>
       </c>
       <c r="I141" s="2">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="J141" s="2">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="K141" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="L141" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="L141" s="26"/>
+      <c r="M141" s="27"/>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B142" t="s">
-        <v>323</v>
+        <v>468</v>
       </c>
       <c r="C142" t="s">
-        <v>322</v>
+        <v>464</v>
       </c>
       <c r="D142">
-        <v>332</v>
+        <v>380</v>
       </c>
       <c r="E142">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F142" s="2">
         <v>1</v>
       </c>
       <c r="G142" s="30">
-        <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]</f>
-        <v>664</v>
-      </c>
-      <c r="H142" s="9" t="s">
+        <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
+        <v>2280</v>
+      </c>
+      <c r="H142" t="s">
         <v>275</v>
       </c>
       <c r="I142" s="2">
         <v>0.8</v>
       </c>
       <c r="J142" s="2">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="K142" s="2">
-        <v>1.1499999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="L142" s="15"/>
-      <c r="O142" t="s">
-        <v>281</v>
-      </c>
+      <c r="M142" s="12"/>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>333</v>
       </c>
       <c r="B143" t="s">
-        <v>324</v>
+        <v>359</v>
       </c>
       <c r="C143" t="s">
-        <v>322</v>
+        <v>360</v>
       </c>
       <c r="D143">
-        <v>276</v>
+        <v>173</v>
       </c>
       <c r="E143">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F143" s="2">
         <v>1</v>
       </c>
       <c r="G143" s="30">
-        <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]</f>
-        <v>552</v>
-      </c>
-      <c r="H143" s="9" t="s">
+        <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
+        <v>2595</v>
+      </c>
+      <c r="H143" t="s">
         <v>275</v>
       </c>
       <c r="I143" s="2">
@@ -12815,126 +12988,118 @@
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>173</v>
+        <v>333</v>
       </c>
       <c r="B144" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C144" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="D144">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E144">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F144" s="2">
         <v>1</v>
       </c>
       <c r="G144" s="30">
-        <v>350</v>
-      </c>
-      <c r="H144" s="9" t="s">
-        <v>49</v>
+        <v>800</v>
+      </c>
+      <c r="H144" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="I144" s="2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="J144" s="2">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K144" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="L144"/>
-      <c r="M144"/>
-      <c r="N144"/>
+        <v>0.9</v>
+      </c>
+      <c r="L144" s="15"/>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>173</v>
+        <v>333</v>
       </c>
       <c r="B145" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C145" t="s">
-        <v>175</v>
+        <v>322</v>
       </c>
       <c r="D145">
-        <v>48</v>
+        <v>332</v>
       </c>
       <c r="E145">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F145" s="2">
         <v>1</v>
       </c>
       <c r="G145" s="30">
-        <v>288</v>
-      </c>
-      <c r="H145" s="10" t="s">
-        <v>329</v>
+        <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]</f>
+        <v>664</v>
+      </c>
+      <c r="H145" s="9" t="s">
+        <v>275</v>
       </c>
       <c r="I145" s="2">
         <v>0.8</v>
       </c>
       <c r="J145" s="2">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="K145" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="L145"/>
-      <c r="M145"/>
-      <c r="N145"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L145" s="15"/>
       <c r="O145" t="s">
-        <v>331</v>
+        <v>281</v>
       </c>
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>173</v>
+        <v>333</v>
       </c>
       <c r="B146" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C146" t="s">
-        <v>180</v>
+        <v>322</v>
       </c>
       <c r="D146">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="E146">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F146" s="2">
         <v>1</v>
       </c>
       <c r="G146" s="30">
-        <v>240</v>
-      </c>
-      <c r="H146" s="13" t="s">
-        <v>330</v>
+        <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]</f>
+        <v>552</v>
+      </c>
+      <c r="H146" s="9" t="s">
+        <v>275</v>
       </c>
       <c r="I146" s="2">
         <v>0.8</v>
       </c>
       <c r="J146" s="2">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="K146" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="L146" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M146" s="27">
-        <v>2</v>
-      </c>
-      <c r="N146"/>
+        <v>1</v>
+      </c>
+      <c r="L146" s="15"/>
       <c r="O146" t="s">
-        <v>472</v>
+        <v>281</v>
       </c>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.3">
@@ -12942,23 +13107,22 @@
         <v>173</v>
       </c>
       <c r="B147" t="s">
-        <v>454</v>
+        <v>325</v>
       </c>
       <c r="C147" t="s">
-        <v>447</v>
+        <v>328</v>
       </c>
       <c r="D147">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E147">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F147" s="2">
         <v>1</v>
       </c>
       <c r="G147" s="30">
-        <f>Barrage4[[#This Row],[Coefficient]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Base Damage]]</f>
-        <v>600</v>
+        <v>350</v>
       </c>
       <c r="H147" s="9" t="s">
         <v>49</v>
@@ -12972,106 +13136,219 @@
       <c r="K147" s="2">
         <v>1.3</v>
       </c>
-      <c r="L147" s="15"/>
+      <c r="L147"/>
+      <c r="M147"/>
+      <c r="N147"/>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>173</v>
       </c>
       <c r="B148" t="s">
-        <v>455</v>
+        <v>326</v>
       </c>
       <c r="C148" t="s">
-        <v>453</v>
+        <v>175</v>
       </c>
       <c r="D148">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E148">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F148" s="2">
         <v>1</v>
       </c>
       <c r="G148" s="30">
-        <f>Barrage4[[#This Row],[Coefficient]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Base Damage]]</f>
-        <v>432</v>
-      </c>
-      <c r="H148" s="9" t="s">
-        <v>49</v>
+        <v>288</v>
+      </c>
+      <c r="H148" s="10" t="s">
+        <v>329</v>
       </c>
       <c r="I148" s="2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J148" s="2">
         <v>1</v>
       </c>
       <c r="K148" s="2">
-        <v>1</v>
-      </c>
-      <c r="L148" s="15"/>
+        <v>1.3</v>
+      </c>
+      <c r="L148"/>
+      <c r="M148"/>
+      <c r="N148"/>
+      <c r="O148" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>173</v>
       </c>
       <c r="B149" t="s">
+        <v>327</v>
+      </c>
+      <c r="C149" t="s">
+        <v>180</v>
+      </c>
+      <c r="D149">
+        <v>40</v>
+      </c>
+      <c r="E149">
+        <v>6</v>
+      </c>
+      <c r="F149" s="2">
+        <v>1</v>
+      </c>
+      <c r="G149" s="30">
+        <v>240</v>
+      </c>
+      <c r="H149" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="I149" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J149" s="2">
+        <v>1</v>
+      </c>
+      <c r="K149" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="L149" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="M149" s="27">
+        <v>2</v>
+      </c>
+      <c r="N149"/>
+      <c r="O149" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>173</v>
+      </c>
+      <c r="B150" t="s">
+        <v>454</v>
+      </c>
+      <c r="C150" t="s">
+        <v>447</v>
+      </c>
+      <c r="D150">
+        <v>60</v>
+      </c>
+      <c r="E150">
+        <v>10</v>
+      </c>
+      <c r="F150" s="2">
+        <v>1</v>
+      </c>
+      <c r="G150" s="30">
+        <f>Barrage4[[#This Row],[Coefficient]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Base Damage]]</f>
+        <v>600</v>
+      </c>
+      <c r="H150" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I150" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J150" s="2">
+        <v>1</v>
+      </c>
+      <c r="K150" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="L150" s="15"/>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>173</v>
+      </c>
+      <c r="B151" t="s">
+        <v>455</v>
+      </c>
+      <c r="C151" t="s">
+        <v>453</v>
+      </c>
+      <c r="D151">
+        <v>36</v>
+      </c>
+      <c r="E151">
+        <v>12</v>
+      </c>
+      <c r="F151" s="2">
+        <v>1</v>
+      </c>
+      <c r="G151" s="30">
+        <f>Barrage4[[#This Row],[Coefficient]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Base Damage]]</f>
+        <v>432</v>
+      </c>
+      <c r="H151" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I151" s="2">
+        <v>1</v>
+      </c>
+      <c r="J151" s="2">
+        <v>1</v>
+      </c>
+      <c r="K151" s="2">
+        <v>1</v>
+      </c>
+      <c r="L151" s="15"/>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>173</v>
+      </c>
+      <c r="B152" t="s">
         <v>467</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C152" t="s">
         <v>461</v>
       </c>
-      <c r="D149">
+      <c r="D152">
         <v>36</v>
       </c>
-      <c r="E149">
+      <c r="E152">
         <v>7</v>
       </c>
-      <c r="F149" s="2">
-        <v>1</v>
-      </c>
-      <c r="G149" s="30">
+      <c r="F152" s="2">
+        <v>1</v>
+      </c>
+      <c r="G152" s="30">
         <f>Barrage4[[#This Row],[Coefficient]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Base Damage]]</f>
         <v>252</v>
       </c>
-      <c r="H149" s="9" t="s">
+      <c r="H152" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I149" s="2">
+      <c r="I152" s="2">
         <v>0.8</v>
       </c>
-      <c r="J149" s="2">
-        <v>1</v>
-      </c>
-      <c r="K149" s="2">
+      <c r="J152" s="2">
+        <v>1</v>
+      </c>
+      <c r="K152" s="2">
         <v>1.3</v>
       </c>
-      <c r="L149" s="32"/>
-      <c r="M149" s="33"/>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B150" s="36"/>
-      <c r="G150" s="30"/>
-      <c r="H150" s="13"/>
-      <c r="L150" s="15"/>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L151" s="15"/>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H152" s="13"/>
-      <c r="L152" s="15"/>
+      <c r="L152" s="32"/>
+      <c r="M152" s="33"/>
     </row>
     <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B153" s="36"/>
+      <c r="G153" s="30"/>
       <c r="H153" s="13"/>
       <c r="L153" s="15"/>
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H154" s="13"/>
       <c r="L154" s="15"/>
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H155" s="10"/>
+      <c r="H155" s="13"/>
       <c r="L155" s="15"/>
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.3">
@@ -13083,62 +13360,26 @@
       <c r="L157" s="15"/>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I158"/>
+      <c r="H158" s="10"/>
       <c r="L158" s="15"/>
-      <c r="M158" s="12"/>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I159"/>
+      <c r="H159" s="13"/>
       <c r="L159" s="15"/>
-      <c r="M159" s="12"/>
-    </row>
-    <row r="160" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A160"/>
-      <c r="B160"/>
-      <c r="C160"/>
-      <c r="D160"/>
-      <c r="E160"/>
-      <c r="F160" s="2"/>
-      <c r="G160" s="29"/>
-      <c r="H160"/>
-      <c r="I160"/>
-      <c r="J160" s="2"/>
-      <c r="K160" s="2"/>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H160" s="13"/>
       <c r="L160" s="15"/>
-      <c r="M160" s="12"/>
-      <c r="O160"/>
-    </row>
-    <row r="161" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A161"/>
-      <c r="B161"/>
-      <c r="C161"/>
-      <c r="D161"/>
-      <c r="E161"/>
-      <c r="F161" s="2"/>
-      <c r="G161" s="29"/>
-      <c r="H161"/>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I161"/>
-      <c r="J161" s="2"/>
-      <c r="K161" s="2"/>
       <c r="L161" s="15"/>
       <c r="M161" s="12"/>
-      <c r="O161"/>
-    </row>
-    <row r="162" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A162"/>
-      <c r="B162"/>
-      <c r="C162"/>
-      <c r="D162"/>
-      <c r="E162"/>
-      <c r="F162" s="2"/>
-      <c r="G162" s="29"/>
-      <c r="H162"/>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I162"/>
-      <c r="J162" s="2"/>
-      <c r="K162" s="2"/>
       <c r="L162" s="15"/>
       <c r="M162" s="12"/>
-      <c r="O162"/>
     </row>
     <row r="163" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163"/>
@@ -13164,7 +13405,7 @@
       <c r="E164"/>
       <c r="F164" s="2"/>
       <c r="G164" s="29"/>
-      <c r="H164" s="13"/>
+      <c r="H164"/>
       <c r="I164"/>
       <c r="J164" s="2"/>
       <c r="K164" s="2"/>
@@ -13200,9 +13441,57 @@
       <c r="I166"/>
       <c r="J166" s="2"/>
       <c r="K166" s="2"/>
-      <c r="L166" s="2"/>
+      <c r="L166" s="15"/>
       <c r="M166" s="12"/>
       <c r="O166"/>
+    </row>
+    <row r="167" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A167"/>
+      <c r="B167"/>
+      <c r="C167"/>
+      <c r="D167"/>
+      <c r="E167"/>
+      <c r="F167" s="2"/>
+      <c r="G167" s="29"/>
+      <c r="H167" s="13"/>
+      <c r="I167"/>
+      <c r="J167" s="2"/>
+      <c r="K167" s="2"/>
+      <c r="L167" s="15"/>
+      <c r="M167" s="12"/>
+      <c r="O167"/>
+    </row>
+    <row r="168" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A168"/>
+      <c r="B168"/>
+      <c r="C168"/>
+      <c r="D168"/>
+      <c r="E168"/>
+      <c r="F168" s="2"/>
+      <c r="G168" s="29"/>
+      <c r="H168"/>
+      <c r="I168"/>
+      <c r="J168" s="2"/>
+      <c r="K168" s="2"/>
+      <c r="L168" s="15"/>
+      <c r="M168" s="12"/>
+      <c r="O168"/>
+    </row>
+    <row r="169" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A169"/>
+      <c r="B169"/>
+      <c r="C169"/>
+      <c r="D169"/>
+      <c r="E169"/>
+      <c r="F169" s="2"/>
+      <c r="G169" s="29"/>
+      <c r="H169"/>
+      <c r="I169"/>
+      <c r="J169" s="2"/>
+      <c r="K169" s="2"/>
+      <c r="L169" s="2"/>
+      <c r="M169" s="12"/>
+      <c r="O169"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
@@ -13278,7 +13567,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G98:G127">
+  <conditionalFormatting sqref="G98:G130">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -13290,7 +13579,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G128:G143">
+  <conditionalFormatting sqref="G131:G146">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -13302,7 +13591,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G144:G149">
+  <conditionalFormatting sqref="G147:G152">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -13314,7 +13603,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G128:G139">
+  <conditionalFormatting sqref="G131:G142">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -13326,7 +13615,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G140:G143">
+  <conditionalFormatting sqref="G143:G146">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Hololive - Translated/Updated Skills
</commit_message>
<xml_diff>
--- a/BarrageChart.xlsx
+++ b/BarrageChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SICA\Pictures\AL\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF90FEE-BA6A-48A2-A934-706F0C444E8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94DE722-CE00-499B-8A08-9671DE761178}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Skill Barrages" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="529">
   <si>
     <t>Barrage Name (Skill Level 2)</t>
   </si>
@@ -1558,30 +1559,15 @@
     <t>Shirakami Fubuki</t>
   </si>
   <si>
-    <t>500lb</t>
-  </si>
-  <si>
     <t>60% Torpedo Stat</t>
   </si>
   <si>
     <t>Natsuiro Matsuri</t>
   </si>
   <si>
-    <t xml:space="preserve">
-与你眺望的夏日之花</t>
-  </si>
-  <si>
     <t>Minato Aqua</t>
   </si>
   <si>
-    <t xml:space="preserve">
-向日葵的约定</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-阿修罗修罗刹鬼神斩</t>
-  </si>
-  <si>
     <t>Nakiri Ayame</t>
   </si>
   <si>
@@ -1589,10 +1575,6 @@
   </si>
   <si>
     <t>AOE, 120 Range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-MP清零的「EXPLOSION」</t>
   </si>
   <si>
     <t>Murasaki Shion</t>
@@ -1611,16 +1593,34 @@
 Dream☆Story</t>
   </si>
   <si>
-    <t>野性的二元论 TP</t>
-  </si>
-  <si>
     <t>Ookami Mio</t>
   </si>
   <si>
-    <t>野性的二元论 Bomb</t>
-  </si>
-  <si>
-    <t>向日葵的约定 Enhanced</t>
+    <t>Promise to the Sunflower</t>
+  </si>
+  <si>
+    <t>Promise to the Sunflower Enhanced</t>
+  </si>
+  <si>
+    <t>MP Burst - Explosion</t>
+  </si>
+  <si>
+    <t>Wild Dualism TP</t>
+  </si>
+  <si>
+    <t>Wild Dualism Bomb</t>
+  </si>
+  <si>
+    <t>The Summer Flower We Watch AP</t>
+  </si>
+  <si>
+    <t>The Summer Flower We Watch HE</t>
+  </si>
+  <si>
+    <t>Ashura Shura Demon-god Killing Slash</t>
+  </si>
+  <si>
+    <t>Mach 2.42 Blossom</t>
   </si>
 </sst>
 </file>
@@ -1630,7 +1630,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1756,12 +1756,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF777777"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1820,7 +1814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1885,12 +1879,11 @@
     <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7374,8 +7367,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D139" workbookViewId="0">
-      <selection activeCell="P159" sqref="P159"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8229,7 +8222,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>508</v>
+        <v>528</v>
       </c>
       <c r="C22" t="s">
         <v>507</v>
@@ -8263,18 +8256,18 @@
       <c r="M22" s="12"/>
       <c r="N22" s="17"/>
       <c r="O22" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="40" t="s">
-        <v>511</v>
+      <c r="B23" t="s">
+        <v>525</v>
       </c>
       <c r="C23" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D23">
         <v>24</v>
@@ -8311,11 +8304,11 @@
       <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="40" t="s">
-        <v>511</v>
+      <c r="B24" t="s">
+        <v>526</v>
       </c>
       <c r="C24" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D24">
         <v>24</v>
@@ -9094,10 +9087,10 @@
         <v>132</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>514</v>
+        <v>527</v>
       </c>
       <c r="C44" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D44">
         <v>81</v>
@@ -9113,7 +9106,7 @@
         <v>81</v>
       </c>
       <c r="H44" s="20" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="I44" s="2">
         <v>1</v>
@@ -9129,7 +9122,7 @@
         <v>20</v>
       </c>
       <c r="O44" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -12674,10 +12667,10 @@
         <v>272</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="C135" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="D135">
         <v>122</v>
@@ -12714,10 +12707,10 @@
         <v>272</v>
       </c>
       <c r="B136" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C136" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="D136">
         <v>240</v>
@@ -12754,10 +12747,10 @@
         <v>272</v>
       </c>
       <c r="B137" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C137" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="D137">
         <v>300</v>
@@ -13260,11 +13253,11 @@
       <c r="A150" t="s">
         <v>332</v>
       </c>
-      <c r="B150" s="40" t="s">
-        <v>518</v>
+      <c r="B150" s="3" t="s">
+        <v>522</v>
       </c>
       <c r="C150" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="D150">
         <v>245</v>
@@ -13280,7 +13273,7 @@
         <v>245</v>
       </c>
       <c r="H150" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="I150" s="2">
         <v>1</v>
@@ -13294,7 +13287,7 @@
       <c r="L150" s="15"/>
       <c r="M150" s="12"/>
       <c r="O150" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.3">
@@ -13693,11 +13686,11 @@
       <c r="A161" t="s">
         <v>173</v>
       </c>
-      <c r="B161" s="41" t="s">
-        <v>513</v>
+      <c r="B161" t="s">
+        <v>520</v>
       </c>
       <c r="C161" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D161">
         <v>60</v>
@@ -13733,11 +13726,11 @@
       <c r="A162" t="s">
         <v>173</v>
       </c>
-      <c r="B162" s="41" t="s">
-        <v>527</v>
+      <c r="B162" t="s">
+        <v>521</v>
       </c>
       <c r="C162" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D162">
         <v>60</v>

</xml_diff>

<commit_message>
Updated Sora's barrage/fixed some typos
</commit_message>
<xml_diff>
--- a/BarrageChart.xlsx
+++ b/BarrageChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SICA\Pictures\AL\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94DE722-CE00-499B-8A08-9671DE761178}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDAF4C4-980E-44A4-992A-D43C6EA8DD11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Skill Barrages" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="531">
   <si>
     <t>Barrage Name (Skill Level 2)</t>
   </si>
@@ -1621,16 +1620,23 @@
   </si>
   <si>
     <t>Mach 2.42 Blossom</t>
+  </si>
+  <si>
+    <t>Admiral Hipper Muse Barrage</t>
+  </si>
+  <si>
+    <t>Admiral Hipper Muse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1782,6 +1788,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1814,7 +1834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1884,6 +1904,9 @@
     <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2025,8 +2048,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Barrage" displayName="Barrage" ref="A1:O129" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:O129" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Barrage" displayName="Barrage" ref="A1:O130" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:O130" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Type"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Barrage Name (Skill Level 2)"/>
@@ -2336,10 +2359,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O129"/>
+  <dimension ref="A1:O130"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="G124" sqref="G124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6764,7 +6787,7 @@
         <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
         <v>240</v>
       </c>
-      <c r="H115" t="s">
+      <c r="H115" s="39" t="s">
         <v>477</v>
       </c>
       <c r="I115" s="2">
@@ -6783,62 +6806,67 @@
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="B116" t="s">
-        <v>450</v>
+        <v>529</v>
       </c>
       <c r="C116" t="s">
-        <v>451</v>
+        <v>530</v>
       </c>
       <c r="D116">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="E116">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F116" s="2">
         <v>1</v>
       </c>
       <c r="G116" s="30">
-        <v>360</v>
-      </c>
-      <c r="H116" t="s">
-        <v>49</v>
+        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
+        <v>420</v>
+      </c>
+      <c r="H116" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="I116" s="2">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J116" s="2">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="K116" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="L116" s="15"/>
-      <c r="M116" s="12"/>
+        <v>1</v>
+      </c>
+      <c r="L116" s="41">
+        <v>0.08</v>
+      </c>
+      <c r="M116" s="42">
+        <v>3</v>
+      </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>173</v>
       </c>
       <c r="B117" t="s">
-        <v>174</v>
+        <v>450</v>
       </c>
       <c r="C117" t="s">
-        <v>175</v>
+        <v>451</v>
       </c>
       <c r="D117">
         <v>60</v>
       </c>
       <c r="E117">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F117" s="2">
         <v>1</v>
       </c>
       <c r="G117" s="30">
-        <v>540</v>
+        <v>360</v>
       </c>
       <c r="H117" t="s">
         <v>49</v>
@@ -6860,10 +6888,10 @@
         <v>173</v>
       </c>
       <c r="B118" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C118" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D118">
         <v>60</v>
@@ -6897,22 +6925,22 @@
         <v>173</v>
       </c>
       <c r="B119" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C119" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D119">
         <v>60</v>
       </c>
       <c r="E119">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F119" s="2">
         <v>1</v>
       </c>
       <c r="G119" s="30">
-        <v>360</v>
+        <v>540</v>
       </c>
       <c r="H119" t="s">
         <v>49</v>
@@ -6934,13 +6962,13 @@
         <v>173</v>
       </c>
       <c r="B120" t="s">
-        <v>413</v>
+        <v>182</v>
       </c>
       <c r="C120" t="s">
-        <v>414</v>
+        <v>177</v>
       </c>
       <c r="D120">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E120">
         <v>6</v>
@@ -6949,8 +6977,7 @@
         <v>1</v>
       </c>
       <c r="G120" s="30">
-        <f>55*6</f>
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="H120" t="s">
         <v>49</v>
@@ -6964,21 +6991,21 @@
       <c r="K120" s="2">
         <v>1.3</v>
       </c>
-      <c r="L120" s="26"/>
-      <c r="M120" s="28"/>
+      <c r="L120" s="15"/>
+      <c r="M120" s="12"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>173</v>
       </c>
       <c r="B121" t="s">
-        <v>183</v>
+        <v>413</v>
       </c>
       <c r="C121" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D121">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E121">
         <v>6</v>
@@ -6987,7 +7014,8 @@
         <v>1</v>
       </c>
       <c r="G121" s="30">
-        <v>360</v>
+        <f>55*6</f>
+        <v>330</v>
       </c>
       <c r="H121" t="s">
         <v>49</v>
@@ -7001,30 +7029,30 @@
       <c r="K121" s="2">
         <v>1.3</v>
       </c>
-      <c r="L121" s="15"/>
-      <c r="M121" s="12"/>
+      <c r="L121" s="26"/>
+      <c r="M121" s="28"/>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>173</v>
       </c>
       <c r="B122" t="s">
-        <v>447</v>
+        <v>183</v>
       </c>
       <c r="C122" t="s">
-        <v>178</v>
+        <v>412</v>
       </c>
       <c r="D122">
         <v>60</v>
       </c>
       <c r="E122">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F122" s="2">
         <v>1</v>
       </c>
       <c r="G122" s="30">
-        <v>540</v>
+        <v>360</v>
       </c>
       <c r="H122" t="s">
         <v>49</v>
@@ -7046,101 +7074,100 @@
         <v>173</v>
       </c>
       <c r="B123" t="s">
-        <v>184</v>
+        <v>447</v>
       </c>
       <c r="C123" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D123">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="E123">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F123" s="2">
         <v>1</v>
       </c>
       <c r="G123" s="30">
-        <v>600</v>
-      </c>
-      <c r="H123" s="13" t="s">
-        <v>33</v>
+        <v>540</v>
+      </c>
+      <c r="H123" t="s">
+        <v>49</v>
       </c>
       <c r="I123" s="2">
-        <v>1.25</v>
+        <v>0.8</v>
       </c>
       <c r="J123" s="2">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="K123" s="2">
-        <v>0.65</v>
-      </c>
-      <c r="L123" s="15">
-        <v>0.08</v>
-      </c>
-      <c r="M123" s="12">
-        <v>3</v>
-      </c>
+        <v>1.3</v>
+      </c>
+      <c r="L123" s="15"/>
+      <c r="M123" s="12"/>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>173</v>
       </c>
       <c r="B124" t="s">
-        <v>462</v>
+        <v>184</v>
       </c>
       <c r="C124" t="s">
-        <v>461</v>
+        <v>179</v>
       </c>
       <c r="D124">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="E124">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F124" s="2">
         <v>1</v>
       </c>
       <c r="G124" s="30">
-        <v>576</v>
-      </c>
-      <c r="H124" t="s">
-        <v>49</v>
+        <v>600</v>
+      </c>
+      <c r="H124" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="I124" s="2">
-        <v>0.8</v>
+        <v>1.25</v>
       </c>
       <c r="J124" s="2">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="K124" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="L124" s="15"/>
-      <c r="M124" s="12"/>
+        <v>0.65</v>
+      </c>
+      <c r="L124" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="M124" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>173</v>
       </c>
       <c r="B125" t="s">
-        <v>366</v>
+        <v>462</v>
       </c>
       <c r="C125" t="s">
-        <v>367</v>
+        <v>461</v>
       </c>
       <c r="D125">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E125">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F125" s="2">
         <v>1</v>
       </c>
       <c r="G125" s="30">
-        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>495</v>
+        <v>576</v>
       </c>
       <c r="H125" t="s">
         <v>49</v>
@@ -7154,21 +7181,21 @@
       <c r="K125" s="2">
         <v>1.3</v>
       </c>
-      <c r="L125" s="23"/>
-      <c r="M125" s="25"/>
+      <c r="L125" s="15"/>
+      <c r="M125" s="12"/>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>173</v>
       </c>
       <c r="B126" t="s">
-        <v>444</v>
+        <v>366</v>
       </c>
       <c r="C126" t="s">
-        <v>443</v>
+        <v>367</v>
       </c>
       <c r="D126">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E126">
         <v>9</v>
@@ -7178,7 +7205,7 @@
       </c>
       <c r="G126" s="30">
         <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>540</v>
+        <v>495</v>
       </c>
       <c r="H126" t="s">
         <v>49</v>
@@ -7192,17 +7219,18 @@
       <c r="K126" s="2">
         <v>1.3</v>
       </c>
-      <c r="L126" s="15"/>
+      <c r="L126" s="23"/>
+      <c r="M126" s="25"/>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>173</v>
       </c>
       <c r="B127" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C127" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D127">
         <v>60</v>
@@ -7236,23 +7264,23 @@
         <v>173</v>
       </c>
       <c r="B128" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C128" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D128">
         <v>60</v>
       </c>
       <c r="E128">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F128" s="2">
         <v>1</v>
       </c>
       <c r="G128" s="30">
         <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
-        <v>360</v>
+        <v>540</v>
       </c>
       <c r="H128" t="s">
         <v>49</v>
@@ -7273,10 +7301,10 @@
         <v>173</v>
       </c>
       <c r="B129" t="s">
-        <v>491</v>
+        <v>448</v>
       </c>
       <c r="C129" t="s">
-        <v>492</v>
+        <v>449</v>
       </c>
       <c r="D129">
         <v>60</v>
@@ -7304,6 +7332,43 @@
         <v>1.3</v>
       </c>
       <c r="L129" s="15"/>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>173</v>
+      </c>
+      <c r="B130" t="s">
+        <v>491</v>
+      </c>
+      <c r="C130" t="s">
+        <v>492</v>
+      </c>
+      <c r="D130">
+        <v>60</v>
+      </c>
+      <c r="E130">
+        <v>6</v>
+      </c>
+      <c r="F130" s="2">
+        <v>1</v>
+      </c>
+      <c r="G130" s="30">
+        <f>Barrage[[#This Row],[Base Damage]]*Barrage[[#This Row],[Total Rounds]]*Barrage[[#This Row],[Coefficient]]</f>
+        <v>360</v>
+      </c>
+      <c r="H130" t="s">
+        <v>49</v>
+      </c>
+      <c r="I130" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J130" s="2">
+        <v>1</v>
+      </c>
+      <c r="K130" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="L130" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G58">
@@ -7330,7 +7395,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G89:G115">
+  <conditionalFormatting sqref="G89:G116">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -7342,7 +7407,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G116:G129">
+  <conditionalFormatting sqref="G117:G130">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -7367,8 +7432,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="F140" sqref="F140"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="H130" sqref="H130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8335,8 +8400,12 @@
       <c r="K24" s="2">
         <v>0.6</v>
       </c>
-      <c r="L24" s="15"/>
-      <c r="M24" s="12"/>
+      <c r="L24" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="M24" s="12">
+        <v>1</v>
+      </c>
       <c r="N24" s="17"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -12676,14 +12745,14 @@
         <v>122</v>
       </c>
       <c r="E135">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F135" s="2">
-        <v>1</v>
+        <v>1.18</v>
       </c>
       <c r="G135" s="30">
         <f>Barrage4[[#This Row],[Base Damage]]*Barrage4[[#This Row],[Total Rounds]]*Barrage4[[#This Row],[Coefficient]]</f>
-        <v>366</v>
+        <v>2159.4</v>
       </c>
       <c r="H135" s="13" t="s">
         <v>33</v>
@@ -12697,7 +12766,12 @@
       <c r="K135" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L135" s="15"/>
+      <c r="L135" s="43">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M135" s="17">
+        <v>1</v>
+      </c>
       <c r="O135" t="s">
         <v>300</v>
       </c>

</xml_diff>